<commit_message>
Resolver Issue and got Bearer Token
</commit_message>
<xml_diff>
--- a/API_Rest_Rangers/src/test/resources/TestData/DataExcel.xlsx
+++ b/API_Rest_Rangers/src/test/resources/TestData/DataExcel.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F366C12A-FA9A-4A7A-B52F-24F6561B3991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A689D83-33AF-40DA-939E-591AEC4C57FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5AAA9EE1-FF49-4EFF-A129-EA93D73D0C52}"/>
   </bookViews>
   <sheets>
-    <sheet name="UserLogin " sheetId="1" r:id="rId1"/>
+    <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Code for Negative Scenario
</commit_message>
<xml_diff>
--- a/API_Rest_Rangers/src/test/resources/TestData/DataExcel.xlsx
+++ b/API_Rest_Rangers/src/test/resources/TestData/DataExcel.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A689D83-33AF-40DA-939E-591AEC4C57FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{94A30E82-9B07-43C7-8206-DBBAB42D922A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5AAA9EE1-FF49-4EFF-A129-EA93D73D0C52}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>userLoginEmail</t>
   </si>
@@ -46,6 +42,12 @@
   </si>
   <si>
     <t>priyankagajbhiye110415@gmail.com</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>XYZ@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -96,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -104,6 +106,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00E7510-94FA-476E-A969-9F8C15F3845C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,9 +450,18 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{5B9CDE09-7714-4142-963F-669869727F44}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{77D591A7-ED0B-45E1-8675-2C0F850EE4CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit with patient Role
</commit_message>
<xml_diff>
--- a/API_Rest_Rangers/src/test/resources/TestData/DataExcel.xlsx
+++ b/API_Rest_Rangers/src/test/resources/TestData/DataExcel.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{36817193-1983-4CBC-B5D7-94A56498949A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{92F7B48F-C0A8-498D-BC35-D0EEDE6729E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{5AAA9EE1-FF49-4EFF-A129-EA93D73D0C52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{5AAA9EE1-FF49-4EFF-A129-EA93D73D0C52}"/>
   </bookViews>
   <sheets>
     <sheet name="UserLogin" sheetId="1" r:id="rId1"/>
     <sheet name="patientInfo1" sheetId="3" r:id="rId2"/>
+    <sheet name="PatientLogin" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M4"/>
+  <oleSize ref="A1:N16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>userLoginEmail</t>
   </si>
@@ -52,6 +53,18 @@
 	"Allergy": "patientInfoAllergyEdit",
 	"FoodCategory": "EGGETARIAN",
 	"DateOfBirth": "2000-11-01"}</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>rams@gmail.com</t>
+  </si>
+  <si>
+    <t>patientpassword</t>
+  </si>
+  <si>
+    <t>patinetEmail</t>
   </si>
 </sst>
 </file>
@@ -431,9 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00E7510-94FA-476E-A969-9F8C15F3845C}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -478,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B65FB2D-E2AE-4571-B985-88189DBF642F}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -500,4 +511,42 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201A26F0-94B7-45FA-8C19-E1BB9B58322F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{989406CD-673C-4883-8DA3-CB41564E4452}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>